<commit_message>
It works! Time to error check
</commit_message>
<xml_diff>
--- a/Exports/2016-10.xlsx
+++ b/Exports/2016-10.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T-Bum\Documents\GitHub\Historical Data\Exports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="21075" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="80" windowWidth="21080" windowHeight="8000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="6">
   <si>
     <t>User</t>
   </si>
@@ -32,11 +37,14 @@
   <si>
     <t>Is Z Done?</t>
   </si>
+  <si>
+    <t>no</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,6 +85,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -125,7 +136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -158,9 +169,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -193,6 +221,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -369,20 +414,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" customWidth="1"/>
+    <col min="3" max="4" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,7 +441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -410,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -424,7 +469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -438,7 +483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -452,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -466,7 +511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -480,7 +525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -494,7 +539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -508,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -522,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -536,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -550,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -558,13 +603,13 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -578,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -592,7 +637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -606,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -620,7 +665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -634,7 +679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -648,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -659,6 +704,930 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
         <v>1</v>
       </c>
     </row>
@@ -673,7 +1642,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -685,7 +1654,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>